<commit_message>
add 905 & 922
</commit_message>
<xml_diff>
--- a/刷题列表.xlsx
+++ b/刷题列表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="163">
   <si>
     <t>分类</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Sort Array By Parity</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/sort-array-by-parity/</t>
   </si>
   <si>
     <t>Sort Array By Parity II</t>
@@ -511,6 +508,10 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/lru-cache/submissions/</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-array-by-parity/</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1102,8 +1103,8 @@
   </sheetPr>
   <dimension ref="A1:F1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1166,7 +1167,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
@@ -1184,7 +1185,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
@@ -1202,7 +1203,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
@@ -1214,13 +1215,13 @@
         <v>16</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
@@ -1234,13 +1235,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>160</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
@@ -1334,7 +1335,7 @@
         <v>31</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
@@ -1472,11 +1473,14 @@
       <c r="C24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>51</v>
+      <c r="D24" s="18" t="s">
+        <v>162</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>9</v>
+        <v>158</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
@@ -1485,13 +1489,16 @@
         <v>6</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="E25" s="10" t="s">
-        <v>9</v>
+        <v>158</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
@@ -1500,10 +1507,10 @@
         <v>6</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>9</v>
@@ -1515,10 +1522,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>9</v>
@@ -1530,10 +1537,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>9</v>
@@ -1545,10 +1552,10 @@
         <v>12</v>
       </c>
       <c r="C29" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>9</v>
@@ -1560,10 +1567,10 @@
         <v>12</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>9</v>
@@ -1575,10 +1582,10 @@
         <v>15</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>9</v>
@@ -1590,10 +1597,10 @@
         <v>12</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>9</v>
@@ -1601,16 +1608,16 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>9</v>
@@ -1622,10 +1629,10 @@
         <v>12</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>72</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>9</v>
@@ -1637,10 +1644,10 @@
         <v>12</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>74</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>9</v>
@@ -1655,7 +1662,7 @@
     </row>
     <row r="37" spans="1:6" ht="21">
       <c r="A37" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -1668,10 +1675,10 @@
         <v>6</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>9</v>
@@ -1684,10 +1691,10 @@
         <v>6</v>
       </c>
       <c r="C39" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>9</v>
@@ -1700,10 +1707,10 @@
         <v>12</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>9</v>
@@ -1716,10 +1723,10 @@
         <v>12</v>
       </c>
       <c r="C41" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>9</v>
@@ -1732,10 +1739,10 @@
         <v>12</v>
       </c>
       <c r="C42" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>9</v>
@@ -1747,10 +1754,10 @@
         <v>12</v>
       </c>
       <c r="C43" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>9</v>
@@ -1762,10 +1769,10 @@
         <v>12</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>9</v>
@@ -1780,7 +1787,7 @@
     </row>
     <row r="46" spans="1:6" ht="21">
       <c r="A46" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -1793,10 +1800,10 @@
         <v>15</v>
       </c>
       <c r="C47" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>9</v>
@@ -1808,10 +1815,10 @@
         <v>15</v>
       </c>
       <c r="C48" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>9</v>
@@ -1823,10 +1830,10 @@
         <v>12</v>
       </c>
       <c r="C49" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>9</v>
@@ -1838,10 +1845,10 @@
         <v>15</v>
       </c>
       <c r="C50" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>9</v>
@@ -1853,10 +1860,10 @@
         <v>12</v>
       </c>
       <c r="C51" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>9</v>
@@ -1872,7 +1879,7 @@
     </row>
     <row r="53" spans="1:6" ht="21">
       <c r="A53" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -1885,10 +1892,10 @@
         <v>12</v>
       </c>
       <c r="C54" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="E54" s="10" t="s">
         <v>9</v>
@@ -1901,10 +1908,10 @@
         <v>12</v>
       </c>
       <c r="C55" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>9</v>
@@ -1916,10 +1923,10 @@
         <v>12</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>9</v>
@@ -1931,10 +1938,10 @@
         <v>15</v>
       </c>
       <c r="C57" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="E57" s="10" t="s">
         <v>9</v>
@@ -1946,10 +1953,10 @@
         <v>12</v>
       </c>
       <c r="C58" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>9</v>
@@ -1964,7 +1971,7 @@
     </row>
     <row r="60" spans="1:6" ht="21">
       <c r="A60" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -1977,10 +1984,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>9</v>
@@ -1993,10 +2000,10 @@
         <v>6</v>
       </c>
       <c r="C62" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>9</v>
@@ -2008,10 +2015,10 @@
         <v>6</v>
       </c>
       <c r="C63" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>9</v>
@@ -2023,10 +2030,10 @@
         <v>12</v>
       </c>
       <c r="C64" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>9</v>
@@ -2038,10 +2045,10 @@
         <v>6</v>
       </c>
       <c r="C65" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>9</v>
@@ -2053,10 +2060,10 @@
         <v>12</v>
       </c>
       <c r="C66" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D66" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>9</v>
@@ -2069,10 +2076,10 @@
         <v>6</v>
       </c>
       <c r="C67" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>126</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>9</v>
@@ -2084,10 +2091,10 @@
         <v>6</v>
       </c>
       <c r="C68" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D68" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="E68" s="10" t="s">
         <v>9</v>
@@ -2099,10 +2106,10 @@
         <v>15</v>
       </c>
       <c r="C69" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="E69" s="10" t="s">
         <v>9</v>
@@ -2114,10 +2121,10 @@
         <v>15</v>
       </c>
       <c r="C70" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D70" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>9</v>
@@ -2130,10 +2137,10 @@
         <v>12</v>
       </c>
       <c r="C71" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>9</v>
@@ -2146,10 +2153,10 @@
         <v>12</v>
       </c>
       <c r="C72" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>9</v>
@@ -2161,10 +2168,10 @@
         <v>12</v>
       </c>
       <c r="C73" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D73" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="E73" s="10" t="str">
         <f>HYPERLINK("https://github.com/haoel/leetcode/blob/master/algorithms/cpp/coinChange/coinChange.cpp","C++")</f>
@@ -2177,10 +2184,10 @@
         <v>12</v>
       </c>
       <c r="C74" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D74" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>9</v>
@@ -2192,10 +2199,10 @@
         <v>15</v>
       </c>
       <c r="C75" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>9</v>
@@ -2207,10 +2214,10 @@
         <v>15</v>
       </c>
       <c r="C76" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D76" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>9</v>
@@ -2222,10 +2229,10 @@
         <v>15</v>
       </c>
       <c r="C77" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D77" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>146</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>9</v>
@@ -2238,10 +2245,10 @@
         <v>15</v>
       </c>
       <c r="C78" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D78" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>9</v>
@@ -2253,10 +2260,10 @@
         <v>12</v>
       </c>
       <c r="C79" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D79" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>9</v>
@@ -2268,10 +2275,10 @@
         <v>12</v>
       </c>
       <c r="C80" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D80" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>9</v>
@@ -2283,10 +2290,10 @@
         <v>6</v>
       </c>
       <c r="C81" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D81" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>9</v>
@@ -2298,10 +2305,10 @@
         <v>12</v>
       </c>
       <c r="C82" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D82" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>9</v>
@@ -2313,10 +2320,10 @@
         <v>12</v>
       </c>
       <c r="C83" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D83" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add 852 & 977
</commit_message>
<xml_diff>
--- a/刷题列表.xlsx
+++ b/刷题列表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="163">
   <si>
     <t>分类</t>
   </si>
@@ -183,19 +183,10 @@
     <t>Squares of a Sorted Array</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/squares-of-a-sorted-array/</t>
-  </si>
-  <si>
     <t>Peak Index in a Mountain Array</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/peak-index-in-a-mountain-array</t>
-  </si>
-  <si>
     <t>Search in Rotated Sorted Array</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/search-in-rotated-sorted-array</t>
   </si>
   <si>
     <t>Search in Rotated Sorted Array II</t>
@@ -512,6 +503,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/sort-array-by-parity/</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/squares-of-a-sorted-array/</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/peak-index-in-a-mountain-array</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-in-rotated-sorted-array</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1103,8 +1106,8 @@
   </sheetPr>
   <dimension ref="A1:F1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1167,7 +1170,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
@@ -1185,7 +1188,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
@@ -1203,7 +1206,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
@@ -1215,13 +1218,13 @@
         <v>16</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
@@ -1235,13 +1238,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
@@ -1335,7 +1338,7 @@
         <v>31</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
@@ -1474,13 +1477,13 @@
         <v>50</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
@@ -1495,10 +1498,10 @@
         <v>52</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
@@ -1509,11 +1512,14 @@
       <c r="C26" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>54</v>
+      <c r="D26" s="18" t="s">
+        <v>160</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>9</v>
+        <v>155</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
@@ -1522,13 +1528,16 @@
         <v>6</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>161</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>9</v>
+        <v>155</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
@@ -1537,10 +1546,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>162</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>9</v>
@@ -1552,10 +1561,10 @@
         <v>12</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>9</v>
@@ -1567,13 +1576,16 @@
         <v>12</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
@@ -1582,13 +1594,16 @@
         <v>15</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
@@ -1597,10 +1612,10 @@
         <v>12</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>9</v>
@@ -1608,16 +1623,16 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>9</v>
@@ -1629,10 +1644,10 @@
         <v>12</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>9</v>
@@ -1644,10 +1659,10 @@
         <v>12</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>9</v>
@@ -1662,7 +1677,7 @@
     </row>
     <row r="37" spans="1:6" ht="21">
       <c r="A37" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -1675,10 +1690,10 @@
         <v>6</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>9</v>
@@ -1691,10 +1706,10 @@
         <v>6</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>9</v>
@@ -1707,10 +1722,10 @@
         <v>12</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>9</v>
@@ -1723,10 +1738,10 @@
         <v>12</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>9</v>
@@ -1739,10 +1754,10 @@
         <v>12</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>9</v>
@@ -1754,10 +1769,10 @@
         <v>12</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>9</v>
@@ -1769,10 +1784,10 @@
         <v>12</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>9</v>
@@ -1787,7 +1802,7 @@
     </row>
     <row r="46" spans="1:6" ht="21">
       <c r="A46" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -1800,10 +1815,10 @@
         <v>15</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>9</v>
@@ -1815,10 +1830,10 @@
         <v>15</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>9</v>
@@ -1830,10 +1845,10 @@
         <v>12</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>9</v>
@@ -1845,10 +1860,10 @@
         <v>15</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>9</v>
@@ -1860,10 +1875,10 @@
         <v>12</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>9</v>
@@ -1879,7 +1894,7 @@
     </row>
     <row r="53" spans="1:6" ht="21">
       <c r="A53" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -1892,10 +1907,10 @@
         <v>12</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E54" s="10" t="s">
         <v>9</v>
@@ -1908,10 +1923,10 @@
         <v>12</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>9</v>
@@ -1923,10 +1938,10 @@
         <v>12</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>9</v>
@@ -1938,10 +1953,10 @@
         <v>15</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E57" s="10" t="s">
         <v>9</v>
@@ -1953,10 +1968,10 @@
         <v>12</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>9</v>
@@ -1971,7 +1986,7 @@
     </row>
     <row r="60" spans="1:6" ht="21">
       <c r="A60" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -1984,10 +1999,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>9</v>
@@ -2000,10 +2015,10 @@
         <v>6</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>9</v>
@@ -2015,10 +2030,10 @@
         <v>6</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>9</v>
@@ -2030,10 +2045,10 @@
         <v>12</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>9</v>
@@ -2045,10 +2060,10 @@
         <v>6</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>9</v>
@@ -2060,10 +2075,10 @@
         <v>12</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>9</v>
@@ -2076,10 +2091,10 @@
         <v>6</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>9</v>
@@ -2091,10 +2106,10 @@
         <v>6</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E68" s="10" t="s">
         <v>9</v>
@@ -2106,10 +2121,10 @@
         <v>15</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E69" s="10" t="s">
         <v>9</v>
@@ -2121,10 +2136,10 @@
         <v>15</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>9</v>
@@ -2137,10 +2152,10 @@
         <v>12</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>9</v>
@@ -2153,10 +2168,10 @@
         <v>12</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>9</v>
@@ -2168,10 +2183,10 @@
         <v>12</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E73" s="10" t="str">
         <f>HYPERLINK("https://github.com/haoel/leetcode/blob/master/algorithms/cpp/coinChange/coinChange.cpp","C++")</f>
@@ -2184,10 +2199,10 @@
         <v>12</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>9</v>
@@ -2199,10 +2214,10 @@
         <v>15</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>9</v>
@@ -2214,10 +2229,10 @@
         <v>15</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>9</v>
@@ -2229,10 +2244,10 @@
         <v>15</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>9</v>
@@ -2245,10 +2260,10 @@
         <v>15</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>9</v>
@@ -2260,10 +2275,10 @@
         <v>12</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>9</v>
@@ -2275,10 +2290,10 @@
         <v>12</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>9</v>
@@ -2290,10 +2305,10 @@
         <v>6</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>9</v>
@@ -2305,10 +2320,10 @@
         <v>12</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>9</v>
@@ -2320,10 +2335,10 @@
         <v>12</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>9</v>

</xml_diff>